<commit_message>
work on hw 6
</commit_message>
<xml_diff>
--- a/hw6/SoftwareComparison.xlsx
+++ b/hw6/SoftwareComparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>R/R Studio</t>
   </si>
@@ -389,7 +389,7 @@
   <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,31 +415,85 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -459,10 +513,28 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first draft of final paper
</commit_message>
<xml_diff>
--- a/hw6/SoftwareComparison.xlsx
+++ b/hw6/SoftwareComparison.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>R/R Studio</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Basic Modeling</t>
   </si>
   <si>
-    <t>Advanced Techniques</t>
-  </si>
-  <si>
     <t>Coding Ability</t>
   </si>
   <si>
@@ -69,14 +66,28 @@
   </si>
   <si>
     <t>Reusability</t>
+  </si>
+  <si>
+    <t>Table 1. Technology Capability Ranked High to Low</t>
+  </si>
+  <si>
+    <t>Advanced Modeling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,143 +413,149 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>